<commit_message>
Sankey app deep transformation. Now works quite well. Start debug N_class for...
</commit_message>
<xml_diff>
--- a/example/GRAFS_data_example_N.xlsx
+++ b/example/GRAFS_data_example_N.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faustega\Documents\These\isterre-dynamic-modeling\grafs-e-project\grafs-e\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D6EBEE-CFAB-456B-92CC-B9713F9625E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0A695C-57A6-4053-BD05-D4669813EE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{F475FEA0-B9E5-4A03-9EDE-4A3E6C5C262C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F475FEA0-B9E5-4A03-9EDE-4A3E6C5C262C}"/>
   </bookViews>
   <sheets>
     <sheet name="Input data" sheetId="2" r:id="rId1"/>
@@ -806,21 +806,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D825A9-0C1C-44E4-98B7-F194F26ABDB6}">
   <dimension ref="A1:E178"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D138" sqref="D138"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="30.81640625" customWidth="1"/>
-    <col min="4" max="4" width="39.1796875" customWidth="1"/>
-    <col min="5" max="5" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+    <col min="4" max="4" width="39.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -837,7 +837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -854,7 +854,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -871,7 +871,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -888,7 +888,7 @@
         <v>2590.69</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -905,7 +905,7 @@
         <v>133.69</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -922,7 +922,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -939,7 +939,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -953,10 +953,10 @@
         <v>58</v>
       </c>
       <c r="E8" s="1">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -973,7 +973,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -990,7 +990,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>19069.295999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>12143.49</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>12834.6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>337.34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>68.27</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>35995.57</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>387.8</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>1301.42</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>2062.46</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>23882</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>5</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>2259100</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>980600</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>1441170</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>33000</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>3997300</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>257750</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>1815490</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>1314680</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>78900</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>12120</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>4998280</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>157750</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>5</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>5</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>5</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>19501008</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>5</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>46.800000000000004</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>5</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>5</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>5</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>5</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>5</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>5</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>5</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>5</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>5</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>5</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>8603000</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>5</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>35.880000000000003</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>5</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>46.800000000000004</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>5</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>5</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>28.999999999999996</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>5</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>5</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>5</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>5</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>5</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>5</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>5</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>5</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>19501008</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>5</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>35.880000000000003</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>5</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>46.800000000000004</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>5</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>5</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>5</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>5</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>5</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>5</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>5</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>5</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>5</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>5</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>8603000</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>5</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>35.880000000000003</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>5</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>46.800000000000004</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>5</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>5</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>28.999999999999996</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>5</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>5</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>5</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>5</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>5</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>5</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>40000000</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>5</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>11.799999999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>5</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>42.5</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>5</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>5</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>5</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>5</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>5</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>70000000</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>5</v>
       </c>
@@ -2384,7 +2384,7 @@
         <v>11.799999999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>5</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>42.5</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>5</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>5</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>5</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>5</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>5</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>5</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>5</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>5</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>5</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>5</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>5</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>5</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>5</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>5</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>5</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>5</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>5</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>5</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>5</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>5</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>5</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>5</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>5</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>5</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>5</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>5</v>
       </c>
@@ -2843,7 +2843,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>5</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>5</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>5</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>5</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>5</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>5</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>5</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>5</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>5</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>5</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>5</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>5</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>5</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>5</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>5</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>5</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>5</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>5</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>5</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>5</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>5</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>5</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>5</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>5</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>5</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>5</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>5</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="10" t="s">
         <v>5</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>2.76</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="11" t="s">
         <v>5</v>
       </c>
@@ -3336,7 +3336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="10" t="s">
         <v>5</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="11" t="s">
         <v>5</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="10" t="s">
         <v>5</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="11" t="s">
         <v>5</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="10" t="s">
         <v>5</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="11" t="s">
         <v>5</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="10" t="s">
         <v>5</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="10" t="s">
         <v>5</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="11" t="s">
         <v>5</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="10" t="s">
         <v>5</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="11" t="s">
         <v>5</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="10" t="s">
         <v>5</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="11" t="s">
         <v>5</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="10" t="s">
         <v>5</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="10" t="s">
         <v>5</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="11" t="s">
         <v>5</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="10" t="s">
         <v>5</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="11" t="s">
         <v>5</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="10" t="s">
         <v>5</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="11" t="s">
         <v>5</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="10" t="s">
         <v>5</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="10" t="s">
         <v>5</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="11" t="s">
         <v>5</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="10" t="s">
         <v>5</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="11" t="s">
         <v>5</v>
       </c>
@@ -3761,7 +3761,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="10" t="s">
         <v>5</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="11" t="s">
         <v>5</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="10" t="s">
         <v>5</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="14" t="s">
         <v>5</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="14" t="s">
         <v>5</v>
       </c>
@@ -3859,16 +3859,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80ABBC0-87F2-4F7A-9036-33771C52D9AC}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.81640625" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>32</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -4099,7 +4099,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -4121,7 +4121,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -4187,7 +4187,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Correction du nom des typologie des cultures (case)
</commit_message>
<xml_diff>
--- a/example/GRAFS_data_example_N.xlsx
+++ b/example/GRAFS_data_example_N.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faustega\Documents\These\isterre-dynamic-modeling\grafs-e-project\grafs-e\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0A695C-57A6-4053-BD05-D4669813EE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9A71AE-DF8B-4C16-A06E-688389372F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F475FEA0-B9E5-4A03-9EDE-4A3E6C5C262C}"/>
+    <workbookView xWindow="16530" yWindow="-15870" windowWidth="25440" windowHeight="15270" xr2:uid="{F475FEA0-B9E5-4A03-9EDE-4A3E6C5C262C}"/>
   </bookViews>
   <sheets>
     <sheet name="Input data" sheetId="2" r:id="rId1"/>
@@ -808,19 +808,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" customWidth="1"/>
-    <col min="4" max="4" width="39.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.81640625" customWidth="1"/>
+    <col min="4" max="4" width="39.1796875" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -837,7 +837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -854,7 +854,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -871,7 +871,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -888,7 +888,7 @@
         <v>2590.69</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -905,7 +905,7 @@
         <v>133.69</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -922,7 +922,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -939,7 +939,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -953,10 +953,10 @@
         <v>58</v>
       </c>
       <c r="E8" s="1">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -973,7 +973,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -990,7 +990,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>19069.295999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>12143.49</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>12834.6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>337.34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>68.27</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>35995.57</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>387.8</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>1301.42</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>2062.46</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>23882</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>5</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>2259100</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>980600</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>1441170</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>33000</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>3997300</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>257750</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
@@ -1293,10 +1293,10 @@
         <v>22</v>
       </c>
       <c r="E28">
-        <v>5000000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>1815490</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>1314680</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>78900</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>12120</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>4998280</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>157750</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>5</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>5</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>5</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>19501008</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>5</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>46.800000000000004</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>5</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>5</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>5</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>5</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>5</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>5</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>5</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>5</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>5</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>5</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>8603000</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>5</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>35.880000000000003</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>5</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>46.800000000000004</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>5</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>5</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>28.999999999999996</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>5</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>5</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>5</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>5</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>5</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>5</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>5</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>5</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>19501008</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>5</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>35.880000000000003</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>5</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>46.800000000000004</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>5</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>5</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>5</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>5</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>5</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>5</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>5</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>5</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>5</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>5</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>8603000</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>5</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>35.880000000000003</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>5</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>46.800000000000004</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>5</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>5</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>28.999999999999996</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>5</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>5</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>5</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>5</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>5</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>5</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>40000000</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>5</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>11.799999999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>5</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>42.5</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>5</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>5</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>5</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>5</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>5</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>70000000</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>5</v>
       </c>
@@ -2384,7 +2384,7 @@
         <v>11.799999999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>5</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>42.5</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>5</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>5</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>5</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="7" t="s">
         <v>5</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>5</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>5</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>5</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>5</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>5</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>5</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>5</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>5</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>5</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>5</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>5</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>5</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>5</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>5</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>5</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>5</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
         <v>5</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>5</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>5</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>5</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>5</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>5</v>
       </c>
@@ -2843,7 +2843,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
         <v>5</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
         <v>5</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
         <v>5</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
         <v>5</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
         <v>5</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
         <v>5</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
         <v>5</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
         <v>5</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
         <v>5</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
         <v>5</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>5</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>5</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>5</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>5</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
         <v>5</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
         <v>5</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
         <v>5</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
         <v>5</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
         <v>5</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
         <v>5</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
         <v>5</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
         <v>5</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
         <v>5</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>5</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
         <v>5</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
         <v>5</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
         <v>5</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="10" t="s">
         <v>5</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>2.76</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="11" t="s">
         <v>5</v>
       </c>
@@ -3336,7 +3336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="10" t="s">
         <v>5</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="11" t="s">
         <v>5</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="10" t="s">
         <v>5</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="11" t="s">
         <v>5</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="10" t="s">
         <v>5</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="11" t="s">
         <v>5</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="10" t="s">
         <v>5</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="10" t="s">
         <v>5</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="11" t="s">
         <v>5</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="10" t="s">
         <v>5</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="11" t="s">
         <v>5</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="10" t="s">
         <v>5</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="11" t="s">
         <v>5</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="10" t="s">
         <v>5</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="10" t="s">
         <v>5</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="11" t="s">
         <v>5</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="10" t="s">
         <v>5</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="11" t="s">
         <v>5</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="10" t="s">
         <v>5</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="11" t="s">
         <v>5</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="10" t="s">
         <v>5</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="10" t="s">
         <v>5</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="11" t="s">
         <v>5</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="10" t="s">
         <v>5</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="11" t="s">
         <v>5</v>
       </c>
@@ -3761,7 +3761,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="10" t="s">
         <v>5</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="11" t="s">
         <v>5</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="10" t="s">
         <v>5</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="14" t="s">
         <v>5</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="14" t="s">
         <v>5</v>
       </c>
@@ -3863,12 +3863,12 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>32</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -4099,7 +4099,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -4121,7 +4121,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -4187,7 +4187,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Suppression de weight import et net import des données d'entrées et du modèle...
</commit_message>
<xml_diff>
--- a/example/GRAFS_data_example_N.xlsx
+++ b/example/GRAFS_data_example_N.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faustega\Documents\These\isterre-dynamic-modeling\grafs-e-project\grafs-e\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9A71AE-DF8B-4C16-A06E-688389372F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8742B4-AD2D-4C99-AC5C-C521D9EACB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16530" yWindow="-15870" windowWidth="25440" windowHeight="15270" xr2:uid="{F475FEA0-B9E5-4A03-9EDE-4A3E6C5C262C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{F475FEA0-B9E5-4A03-9EDE-4A3E6C5C262C}"/>
   </bookViews>
   <sheets>
     <sheet name="Input data" sheetId="2" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="76">
   <si>
     <t>Area</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Seed input (kt seeds/kt Ymax)</t>
   </si>
   <si>
-    <t>Net Import (ktN)</t>
-  </si>
-  <si>
     <t>Diet</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
     <t>Weight diet</t>
   </si>
   <si>
-    <t>Weight import</t>
-  </si>
-  <si>
     <t>Weight distribution</t>
   </si>
   <si>
@@ -282,6 +276,9 @@
   </si>
   <si>
     <t>porcines grasslands excretion</t>
+  </si>
+  <si>
+    <t>Natural meadow forage, Forage</t>
   </si>
 </sst>
 </file>
@@ -804,11 +801,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D825A9-0C1C-44E4-98B7-F194F26ABDB6}">
-  <dimension ref="A1:E178"/>
+  <dimension ref="A1:E174"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -848,7 +845,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E2">
         <v>15000</v>
@@ -865,7 +862,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E3">
         <v>7500</v>
@@ -882,7 +879,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E4">
         <v>2590.69</v>
@@ -899,7 +896,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E5">
         <v>133.69</v>
@@ -916,7 +913,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E6">
         <v>25000</v>
@@ -933,7 +930,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E7" s="1">
         <v>600</v>
@@ -950,7 +947,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E8" s="1">
         <v>10000</v>
@@ -967,7 +964,7 @@
         <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E9">
         <v>1448</v>
@@ -984,7 +981,7 @@
         <v>12</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E10">
         <v>1188</v>
@@ -1018,7 +1015,7 @@
         <v>12</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E12" s="1">
         <v>12143.49</v>
@@ -1035,7 +1032,7 @@
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E13" s="1">
         <v>12834.6</v>
@@ -1052,7 +1049,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E14" s="1">
         <v>337.34</v>
@@ -1069,7 +1066,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E15" s="1">
         <v>68.27</v>
@@ -1086,7 +1083,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E16" s="1">
         <v>35995.57</v>
@@ -1103,7 +1100,7 @@
         <v>12</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E17" s="1">
         <v>387.8</v>
@@ -1120,7 +1117,7 @@
         <v>12</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E18" s="1">
         <v>5000</v>
@@ -1137,7 +1134,7 @@
         <v>12</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E19" s="1">
         <v>1301.42</v>
@@ -1154,7 +1151,7 @@
         <v>12</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E20" s="1">
         <v>2062.46</v>
@@ -1205,7 +1202,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E23" s="1">
         <v>980600</v>
@@ -1324,7 +1321,7 @@
         <v>13</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E30" s="1">
         <v>1314680</v>
@@ -1423,7 +1420,7 @@
         <v>1961</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>14</v>
@@ -1440,7 +1437,7 @@
         <v>1961</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>14</v>
@@ -1491,10 +1488,10 @@
         <v>1961</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E40">
         <v>46.800000000000004</v>
@@ -1508,10 +1505,10 @@
         <v>1961</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E41">
         <v>10</v>
@@ -1525,10 +1522,10 @@
         <v>1961</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E42">
         <v>2.5</v>
@@ -1542,10 +1539,10 @@
         <v>1961</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E43">
         <v>1.25</v>
@@ -1559,10 +1556,10 @@
         <v>1961</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E44">
         <v>10</v>
@@ -1576,10 +1573,10 @@
         <v>1961</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E45">
         <v>0.5</v>
@@ -1593,10 +1590,10 @@
         <v>1961</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E46">
         <v>0.25</v>
@@ -1610,10 +1607,10 @@
         <v>1961</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E47">
         <v>2</v>
@@ -1627,7 +1624,7 @@
         <v>1961</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>15</v>
@@ -1678,10 +1675,10 @@
         <v>1961</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E51">
         <v>35.880000000000003</v>
@@ -1695,10 +1692,10 @@
         <v>1961</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E52" s="1">
         <v>46.800000000000004</v>
@@ -1712,10 +1709,10 @@
         <v>1961</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E53" s="1">
         <v>10</v>
@@ -1729,10 +1726,10 @@
         <v>1961</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E54" s="1">
         <v>28.999999999999996</v>
@@ -1746,10 +1743,10 @@
         <v>1961</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="E55" s="1">
         <v>1</v>
@@ -1763,10 +1760,10 @@
         <v>1961</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E56" s="1">
         <v>10</v>
@@ -1780,10 +1777,10 @@
         <v>1961</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="E57" s="1">
         <v>4</v>
@@ -1797,10 +1794,10 @@
         <v>1961</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E58" s="1">
         <v>0.2</v>
@@ -1814,10 +1811,10 @@
         <v>1961</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E59" s="1">
         <v>2</v>
@@ -1831,7 +1828,7 @@
         <v>2023</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>14</v>
@@ -1882,10 +1879,10 @@
         <v>2023</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E63" s="1">
         <v>35.880000000000003</v>
@@ -1899,10 +1896,10 @@
         <v>2023</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E64" s="1">
         <v>46.800000000000004</v>
@@ -1916,10 +1913,10 @@
         <v>2023</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E65" s="1">
         <v>10</v>
@@ -1933,10 +1930,10 @@
         <v>2023</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E66" s="1">
         <v>2.5</v>
@@ -1950,10 +1947,10 @@
         <v>2023</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E67" s="1">
         <v>1.25</v>
@@ -1967,10 +1964,10 @@
         <v>2023</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E68" s="1">
         <v>10</v>
@@ -1984,10 +1981,10 @@
         <v>2023</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E69" s="1">
         <v>0.5</v>
@@ -2001,10 +1998,10 @@
         <v>2023</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E70" s="1">
         <v>0.25</v>
@@ -2018,10 +2015,10 @@
         <v>2023</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E71" s="1">
         <v>2</v>
@@ -2035,7 +2032,7 @@
         <v>2023</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>15</v>
@@ -2086,10 +2083,10 @@
         <v>2023</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E75">
         <v>35.880000000000003</v>
@@ -2103,10 +2100,10 @@
         <v>2023</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E76" s="1">
         <v>46.800000000000004</v>
@@ -2120,10 +2117,10 @@
         <v>2023</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E77" s="1">
         <v>10</v>
@@ -2137,10 +2134,10 @@
         <v>2023</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E78" s="1">
         <v>28.999999999999996</v>
@@ -2154,10 +2151,10 @@
         <v>2023</v>
       </c>
       <c r="C79" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="E79" s="1">
         <v>1</v>
@@ -2171,10 +2168,10 @@
         <v>2023</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E80" s="1">
         <v>10</v>
@@ -2188,10 +2185,10 @@
         <v>2023</v>
       </c>
       <c r="C81" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="E81" s="1">
         <v>4</v>
@@ -2205,10 +2202,10 @@
         <v>2023</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E82" s="1">
         <v>0.2</v>
@@ -2222,10 +2219,10 @@
         <v>2023</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E83" s="1">
         <v>2</v>
@@ -2256,7 +2253,7 @@
         <v>1961</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>21</v>
@@ -2273,7 +2270,7 @@
         <v>1961</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>21</v>
@@ -2290,7 +2287,7 @@
         <v>1961</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>21</v>
@@ -2324,7 +2321,7 @@
         <v>1961</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>21</v>
@@ -2375,7 +2372,7 @@
         <v>2023</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>21</v>
@@ -2392,7 +2389,7 @@
         <v>2023</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D93" s="5" t="s">
         <v>21</v>
@@ -2409,7 +2406,7 @@
         <v>2023</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D94" s="6" t="s">
         <v>21</v>
@@ -2443,7 +2440,7 @@
         <v>2023</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D96" s="6" t="s">
         <v>21</v>
@@ -2497,7 +2494,7 @@
         <v>23</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E99" s="1">
         <v>40</v>
@@ -2616,7 +2613,7 @@
         <v>23</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E106" s="1">
         <v>40</v>
@@ -2735,7 +2732,7 @@
         <v>24</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E113">
         <v>0.03</v>
@@ -2854,7 +2851,7 @@
         <v>24</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E120">
         <v>0.03</v>
@@ -2953,13 +2950,13 @@
         <v>1961</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E126">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
@@ -2970,13 +2967,13 @@
         <v>2023</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E127">
-        <v>150</v>
+        <v>300</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
@@ -2987,13 +2984,13 @@
         <v>1961</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E128">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
@@ -3004,13 +3001,13 @@
         <v>2023</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E129">
-        <v>300</v>
+        <v>70</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
@@ -3021,13 +3018,13 @@
         <v>1961</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E130">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
@@ -3038,13 +3035,13 @@
         <v>2023</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E131">
-        <v>70</v>
+        <v>8</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
@@ -3055,13 +3052,13 @@
         <v>1961</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E132">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
@@ -3072,13 +3069,13 @@
         <v>2023</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E133">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
@@ -3086,16 +3083,16 @@
         <v>5</v>
       </c>
       <c r="B134">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E134">
-        <v>1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
@@ -3106,13 +3103,13 @@
         <v>1961</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E135">
-        <v>10</v>
+        <v>60</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
@@ -3123,13 +3120,13 @@
         <v>2023</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E136">
-        <v>1</v>
+        <v>60</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
@@ -3140,13 +3137,13 @@
         <v>2023</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E137">
-        <v>0.5</v>
+        <v>25</v>
+      </c>
+      <c r="D137" t="s">
+        <v>14</v>
+      </c>
+      <c r="E137" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
@@ -3157,13 +3154,13 @@
         <v>2023</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E138">
-        <v>0.05</v>
+        <v>25</v>
+      </c>
+      <c r="D138" t="s">
+        <v>15</v>
+      </c>
+      <c r="E138" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
@@ -3171,16 +3168,16 @@
         <v>5</v>
       </c>
       <c r="B139">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>63</v>
+        <v>25</v>
+      </c>
+      <c r="D139" t="s">
+        <v>21</v>
+      </c>
+      <c r="E139" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
@@ -3188,16 +3185,16 @@
         <v>5</v>
       </c>
       <c r="B140">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C140" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D140" t="s">
+        <v>14</v>
+      </c>
+      <c r="E140" t="s">
         <v>36</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
@@ -3205,16 +3202,16 @@
         <v>5</v>
       </c>
       <c r="B141">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D141" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E141" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
@@ -3222,84 +3219,84 @@
         <v>5</v>
       </c>
       <c r="B142">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D142" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E142" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A143" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B143">
-        <v>2023</v>
-      </c>
-      <c r="C143" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D143" t="s">
-        <v>21</v>
-      </c>
-      <c r="E143" t="s">
-        <v>29</v>
+      <c r="A143" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B143" s="2">
+        <v>1961</v>
+      </c>
+      <c r="C143" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D143" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E143" s="9">
+        <v>2.76</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A144" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B144">
-        <v>1961</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D144" t="s">
-        <v>14</v>
-      </c>
-      <c r="E144" t="s">
-        <v>37</v>
+      <c r="A144" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B144" s="3">
+        <v>1961</v>
+      </c>
+      <c r="C144" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D144" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E144" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A145" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B145">
-        <v>1961</v>
-      </c>
-      <c r="C145" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D145" t="s">
-        <v>15</v>
-      </c>
-      <c r="E145" t="s">
-        <v>38</v>
+      <c r="A145" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B145" s="2">
+        <v>1961</v>
+      </c>
+      <c r="C145" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D145" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E145" s="9">
+        <v>2.5</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A146" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B146">
-        <v>1961</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D146" t="s">
-        <v>21</v>
-      </c>
-      <c r="E146" t="s">
-        <v>39</v>
+      <c r="A146" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B146" s="3">
+        <v>1961</v>
+      </c>
+      <c r="C146" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D146" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E146" s="9">
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
@@ -3313,10 +3310,10 @@
         <v>33</v>
       </c>
       <c r="D147" s="5" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="E147" s="9">
-        <v>2.76</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
@@ -3326,14 +3323,14 @@
       <c r="B148" s="3">
         <v>1961</v>
       </c>
-      <c r="C148" s="6" t="s">
+      <c r="C148" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E148" s="9">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="E148" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
@@ -3344,13 +3341,13 @@
         <v>1961</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D149" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E149" s="9">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
@@ -3361,13 +3358,13 @@
         <v>1961</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E150" s="9">
-        <v>2.2000000000000002</v>
+        <v>11</v>
+      </c>
+      <c r="E150" s="12">
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
@@ -3378,80 +3375,80 @@
         <v>1961</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D151" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E151" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A152" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B152" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C152" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D152" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E152" s="9">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A153" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B153" s="3">
+        <v>2023</v>
+      </c>
+      <c r="C153" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D153" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E153" s="9">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A154" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B154" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C154" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D154" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E151" s="9">
+      <c r="E154" s="9">
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A152" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B152" s="3">
-        <v>1961</v>
-      </c>
-      <c r="C152" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D152" s="6" t="s">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A155" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B155" s="3">
+        <v>2023</v>
+      </c>
+      <c r="C155" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D155" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E152" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A153" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B153" s="2">
-        <v>1961</v>
-      </c>
-      <c r="C153" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D153" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E153" s="9">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A154" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B154" s="3">
-        <v>1961</v>
-      </c>
-      <c r="C154" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D154" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E154" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A155" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B155" s="2">
-        <v>1961</v>
-      </c>
-      <c r="C155" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D155" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E155" s="13">
+      <c r="E155" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3463,13 +3460,13 @@
         <v>2023</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E156" s="9">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
@@ -3480,13 +3477,13 @@
         <v>2023</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E157" s="9">
-        <v>2.2000000000000002</v>
+        <v>11</v>
+      </c>
+      <c r="E157" s="12">
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.35">
@@ -3497,81 +3494,81 @@
         <v>2023</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D158" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E158" s="9">
-        <v>2.2000000000000002</v>
+        <v>22</v>
+      </c>
+      <c r="E158" s="13">
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A159" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B159" s="3">
-        <v>2023</v>
+      <c r="A159" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B159" s="2">
+        <v>1961</v>
       </c>
       <c r="C159" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D159" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E159" s="4">
+      <c r="D159" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E159">
         <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A160" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B160" s="2">
-        <v>2023</v>
+      <c r="A160" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B160" s="3">
+        <v>1961</v>
       </c>
       <c r="C160" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D160" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E160" s="9">
-        <v>3.5</v>
+      <c r="D160" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E160">
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A161" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B161" s="3">
-        <v>2023</v>
+      <c r="A161" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B161" s="2">
+        <v>1961</v>
       </c>
       <c r="C161" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D161" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E161" s="12">
+      <c r="D161" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E161">
         <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A162" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B162" s="2">
-        <v>2023</v>
+      <c r="A162" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B162" s="3">
+        <v>1961</v>
       </c>
       <c r="C162" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D162" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E162" s="13">
-        <v>0</v>
+      <c r="D162" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E162">
+        <v>125</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.35">
@@ -3582,10 +3579,10 @@
         <v>1961</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D163" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E163">
         <v>0</v>
@@ -3599,10 +3596,10 @@
         <v>1961</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D164" s="6" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="E164">
         <v>0</v>
@@ -3616,81 +3613,81 @@
         <v>1961</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E165">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A166" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B166" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C166" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D166" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E166">
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A166" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B166" s="3">
-        <v>1961</v>
-      </c>
-      <c r="C166" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D166" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E166">
-        <v>125</v>
-      </c>
-    </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A167" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B167" s="2">
-        <v>1961</v>
+      <c r="A167" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B167" s="3">
+        <v>2023</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D167" s="5" t="s">
-        <v>9</v>
+        <v>34</v>
+      </c>
+      <c r="D167" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="E167">
         <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A168" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B168" s="3">
-        <v>1961</v>
+      <c r="A168" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B168" s="2">
+        <v>2023</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D168" s="6" t="s">
-        <v>11</v>
+        <v>34</v>
+      </c>
+      <c r="D168" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="E168">
         <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A169" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B169" s="2">
-        <v>1961</v>
+      <c r="A169" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B169" s="3">
+        <v>2023</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D169" s="5" t="s">
-        <v>22</v>
+        <v>34</v>
+      </c>
+      <c r="D169" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E169">
-        <v>150</v>
+        <v>125</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.35">
@@ -3701,10 +3698,10 @@
         <v>2023</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D170" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E170">
         <v>0</v>
@@ -3718,10 +3715,10 @@
         <v>2023</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="E171">
         <v>0</v>
@@ -3735,114 +3732,46 @@
         <v>2023</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D172" s="5" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E172">
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A173" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B173" s="3">
-        <v>2023</v>
-      </c>
-      <c r="C173" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D173" s="6" t="s">
-        <v>8</v>
+      <c r="A173" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B173" s="15">
+        <v>1961</v>
+      </c>
+      <c r="C173" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D173" t="s">
+        <v>39</v>
       </c>
       <c r="E173">
-        <v>125</v>
+        <v>20</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A174" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B174" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C174" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D174" s="5" t="s">
-        <v>9</v>
+      <c r="A174" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B174" s="15">
+        <v>2023</v>
+      </c>
+      <c r="C174" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D174" t="s">
+        <v>39</v>
       </c>
       <c r="E174">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A175" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B175" s="3">
-        <v>2023</v>
-      </c>
-      <c r="C175" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D175" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E175">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A176" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B176" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C176" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D176" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E176">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A177" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B177" s="15">
-        <v>1961</v>
-      </c>
-      <c r="C177" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D177" t="s">
-        <v>40</v>
-      </c>
-      <c r="E177">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A178" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B178" s="15">
-        <v>2023</v>
-      </c>
-      <c r="C178" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D178" t="s">
-        <v>40</v>
-      </c>
-      <c r="E178">
         <v>25</v>
       </c>
     </row>
@@ -3859,8 +3788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80ABBC0-87F2-4F7A-9036-33771C52D9AC}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3870,315 +3799,315 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>0.65</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>0.1</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>0.25</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>0.3</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>0.1</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>0.2</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>0.4</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>0.6</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10">
         <v>0.1</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>0.05</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <v>0.1</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <v>0.05</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14">
         <v>0.1</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15">
         <v>0.5</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16">
         <v>0.1</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17">
         <v>0.4</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18">
         <v>0.3</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19">
         <v>0.1</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>0.2</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21">
         <v>0.4</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22">
         <v>0.3</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23">
         <v>0.05</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25">
         <v>0.05</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27">
         <v>0.05</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28">
         <v>0.3</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29">
         <v>0.05</v>
@@ -4189,13 +4118,13 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30">
         <v>0.15</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mecanisms added. Still troubles to explain its behaviour. Debug is ongoing...
</commit_message>
<xml_diff>
--- a/example/GRAFS_data_example_N.xlsx
+++ b/example/GRAFS_data_example_N.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faustega\Documents\These\isterre-dynamic-modeling\grafs-e-project\grafs-e\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8742B4-AD2D-4C99-AC5C-C521D9EACB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32050A34-7E51-414C-8A0B-7749881DEE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{F475FEA0-B9E5-4A03-9EDE-4A3E6C5C262C}"/>
+    <workbookView xWindow="16530" yWindow="-15870" windowWidth="25440" windowHeight="15270" xr2:uid="{F475FEA0-B9E5-4A03-9EDE-4A3E6C5C262C}"/>
   </bookViews>
   <sheets>
     <sheet name="Input data" sheetId="2" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="81">
   <si>
     <t>Area</t>
   </si>
@@ -279,6 +279,21 @@
   </si>
   <si>
     <t>Natural meadow forage, Forage</t>
+  </si>
+  <si>
+    <t>Methanizer_diet</t>
+  </si>
+  <si>
+    <t>bovines slurry, bovines manure, porcines slurry, porcines manure</t>
+  </si>
+  <si>
+    <t>waste</t>
+  </si>
+  <si>
+    <t>Barley grain, Wheat grain, Oats grain, Maize corn</t>
+  </si>
+  <si>
+    <t>Methanizer</t>
   </si>
 </sst>
 </file>
@@ -801,11 +816,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D825A9-0C1C-44E4-98B7-F194F26ABDB6}">
-  <dimension ref="A1:E174"/>
+  <dimension ref="A1:E176"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D130" sqref="D130"/>
+      <selection pane="bottomLeft" activeCell="B143" sqref="B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3232,37 +3247,37 @@
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A143" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B143" s="2">
-        <v>1961</v>
-      </c>
-      <c r="C143" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D143" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E143" s="9">
-        <v>2.76</v>
+      <c r="A143" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B143">
+        <v>1961</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D143" t="s">
+        <v>80</v>
+      </c>
+      <c r="E143" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A144" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B144" s="3">
-        <v>1961</v>
-      </c>
-      <c r="C144" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D144" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E144" s="9">
-        <v>1</v>
+      <c r="A144" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B144">
+        <v>2023</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D144" t="s">
+        <v>80</v>
+      </c>
+      <c r="E144" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
@@ -3273,13 +3288,13 @@
         <v>1961</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="E145" s="9">
-        <v>2.5</v>
+        <v>2.76</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
@@ -3289,14 +3304,14 @@
       <c r="B146" s="3">
         <v>1961</v>
       </c>
-      <c r="C146" s="5" t="s">
-        <v>33</v>
+      <c r="C146" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E146" s="9">
-        <v>2.2000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
@@ -3310,10 +3325,10 @@
         <v>33</v>
       </c>
       <c r="D147" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E147" s="9">
-        <v>2.2000000000000002</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
@@ -3327,10 +3342,10 @@
         <v>33</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E148" s="4">
-        <v>0</v>
+        <v>57</v>
+      </c>
+      <c r="E148" s="9">
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
@@ -3344,10 +3359,10 @@
         <v>33</v>
       </c>
       <c r="D149" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E149" s="9">
-        <v>3.5</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
@@ -3361,9 +3376,9 @@
         <v>33</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E150" s="12">
+        <v>8</v>
+      </c>
+      <c r="E150" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3378,44 +3393,44 @@
         <v>33</v>
       </c>
       <c r="D151" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E151" s="13">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="E151" s="9">
+        <v>3.5</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A152" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B152" s="2">
-        <v>2023</v>
+      <c r="A152" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B152" s="3">
+        <v>1961</v>
       </c>
       <c r="C152" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D152" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E152" s="9">
-        <v>2.5</v>
+      <c r="D152" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E152" s="12">
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A153" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B153" s="3">
-        <v>2023</v>
+      <c r="A153" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B153" s="2">
+        <v>1961</v>
       </c>
       <c r="C153" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D153" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E153" s="9">
-        <v>2.2000000000000002</v>
+      <c r="D153" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E153" s="13">
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
@@ -3429,10 +3444,10 @@
         <v>33</v>
       </c>
       <c r="D154" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E154" s="9">
-        <v>2.2000000000000002</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
@@ -3446,10 +3461,10 @@
         <v>33</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E155" s="4">
-        <v>0</v>
+        <v>57</v>
+      </c>
+      <c r="E155" s="9">
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.35">
@@ -3463,10 +3478,10 @@
         <v>33</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E156" s="9">
-        <v>3.5</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
@@ -3480,9 +3495,9 @@
         <v>33</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E157" s="12">
+        <v>8</v>
+      </c>
+      <c r="E157" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3497,43 +3512,43 @@
         <v>33</v>
       </c>
       <c r="D158" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E158" s="9">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A159" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B159" s="3">
+        <v>2023</v>
+      </c>
+      <c r="C159" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D159" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E159" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A160" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B160" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C160" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D160" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E158" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A159" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B159" s="2">
-        <v>1961</v>
-      </c>
-      <c r="C159" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D159" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E159">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A160" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B160" s="3">
-        <v>1961</v>
-      </c>
-      <c r="C160" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D160" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E160">
+      <c r="E160" s="13">
         <v>0</v>
       </c>
     </row>
@@ -3548,7 +3563,7 @@
         <v>34</v>
       </c>
       <c r="D161" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E161">
         <v>0</v>
@@ -3565,10 +3580,10 @@
         <v>34</v>
       </c>
       <c r="D162" s="6" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="E162">
-        <v>125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.35">
@@ -3582,7 +3597,7 @@
         <v>34</v>
       </c>
       <c r="D163" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E163">
         <v>0</v>
@@ -3599,10 +3614,10 @@
         <v>34</v>
       </c>
       <c r="D164" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E164">
-        <v>0</v>
+        <v>125</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.35">
@@ -3616,44 +3631,44 @@
         <v>34</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E165">
-        <v>150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A166" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B166" s="2">
-        <v>2023</v>
+      <c r="A166" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B166" s="3">
+        <v>1961</v>
       </c>
       <c r="C166" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D166" s="5" t="s">
-        <v>6</v>
+      <c r="D166" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E166">
         <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A167" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B167" s="3">
-        <v>2023</v>
+      <c r="A167" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B167" s="2">
+        <v>1961</v>
       </c>
       <c r="C167" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D167" s="6" t="s">
-        <v>57</v>
+      <c r="D167" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="E167">
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
@@ -3667,7 +3682,7 @@
         <v>34</v>
       </c>
       <c r="D168" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E168">
         <v>0</v>
@@ -3684,10 +3699,10 @@
         <v>34</v>
       </c>
       <c r="D169" s="6" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="E169">
-        <v>125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.35">
@@ -3701,7 +3716,7 @@
         <v>34</v>
       </c>
       <c r="D170" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E170">
         <v>0</v>
@@ -3718,10 +3733,10 @@
         <v>34</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E171">
-        <v>0</v>
+        <v>125</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.35">
@@ -3735,43 +3750,77 @@
         <v>34</v>
       </c>
       <c r="D172" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A173" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B173" s="3">
+        <v>2023</v>
+      </c>
+      <c r="C173" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D173" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A174" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B174" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C174" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D174" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E172">
+      <c r="E174">
         <v>150</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A173" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B173" s="15">
-        <v>1961</v>
-      </c>
-      <c r="C173" s="16" t="s">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A175" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B175" s="15">
+        <v>1961</v>
+      </c>
+      <c r="C175" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D175" t="s">
         <v>39</v>
       </c>
-      <c r="E173">
+      <c r="E175">
         <v>20</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A174" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B174" s="15">
-        <v>2023</v>
-      </c>
-      <c r="C174" s="16" t="s">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A176" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B176" s="15">
+        <v>2023</v>
+      </c>
+      <c r="C176" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D176" t="s">
         <v>39</v>
       </c>
-      <c r="E174">
+      <c r="E176">
         <v>25</v>
       </c>
     </row>
@@ -3786,14 +3835,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80ABBC0-87F2-4F7A-9036-33771C52D9AC}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
     <col min="3" max="3" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4125,6 +4175,50 @@
       </c>
       <c r="C30" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31">
+        <v>0.2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32">
+        <v>0.1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33">
+        <v>0.6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34">
+        <v>0.1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>